<commit_message>
groundwork and implementation of excel sheet parsing/data-placing
</commit_message>
<xml_diff>
--- a/public/excel/PreProduction/QC Documentation.xlsx
+++ b/public/excel/PreProduction/QC Documentation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Part Number:</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>aa</t>
+  </si>
+  <si>
+    <t>${measure1}</t>
   </si>
   <si>
     <t>Visual Attributes</t>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -328,6 +331,9 @@
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -750,92 +756,94 @@
       <c r="B10" s="23">
         <v>121.0</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="C10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25"/>
     </row>
     <row r="11">
       <c r="A11" s="5"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12">
       <c r="A12" s="5"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13">
       <c r="A13" s="5"/>
       <c r="B13" s="23">
         <v>123123.0</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14">
       <c r="A14" s="5"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15">
       <c r="A15" s="5"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16">
       <c r="A16" s="5"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17">
       <c r="A17" s="5"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18">
       <c r="A18" s="5"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19">
       <c r="A19" s="5"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="26" t="s">
-        <v>18</v>
+      <c r="B21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -847,91 +855,91 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="18"/>
       <c r="L22" s="19"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="18"/>
       <c r="L23" s="19"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="18"/>
       <c r="L24" s="19"/>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="18"/>
       <c r="L25" s="19"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="18"/>
       <c r="L26" s="19"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="18"/>
       <c r="L27" s="19"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="18"/>
       <c r="L28" s="19"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="18"/>
       <c r="L29" s="19"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="20"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -1146,7 +1154,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="12"/>
@@ -1183,305 +1191,305 @@
         <v>11</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
     </row>
     <row r="12">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="27"/>
-      <c r="AA12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
     </row>
     <row r="14">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
-      <c r="Z14" s="27"/>
-      <c r="AA14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="27"/>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AA17" s="27"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="27"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="27"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1511,8 +1519,8 @@
       <c r="AA20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1599,7 +1607,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="30"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2147,9 +2155,9 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="1"/>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -2179,9 +2187,9 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="1"/>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
@@ -2209,9 +2217,9 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2239,9 +2247,9 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2295,7 +2303,7 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="12"/>
@@ -2328,10 +2336,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
further optimazations to backend and frontend
</commit_message>
<xml_diff>
--- a/public/excel/PreProduction/QC Documentation.xlsx
+++ b/public/excel/PreProduction/QC Documentation.xlsx
@@ -20,93 +20,201 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+  <si>
+    <t>Par Name:</t>
+  </si>
+  <si>
+    <t>${partName}</t>
+  </si>
+  <si>
+    <t>REV 5-10-21</t>
+  </si>
+  <si>
+    <t>Part Revision:</t>
+  </si>
+  <si>
+    <t>${partRevision}</t>
+  </si>
+  <si>
+    <t>Job #:</t>
+  </si>
+  <si>
+    <t>${jobNumber}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Approval: </t>
+  </si>
+  <si>
+    <t>${firstApproval}</t>
+  </si>
+  <si>
+    <t>Check Freq:</t>
+  </si>
+  <si>
+    <t>${checkFreq}</t>
+  </si>
+  <si>
+    <t>Measurable Attributes</t>
+  </si>
+  <si>
+    <t>Thousanths</t>
+  </si>
+  <si>
+    <t>Skid number &amp; time</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>MIN -</t>
+  </si>
+  <si>
+    <t>Measure=</t>
+  </si>
+  <si>
+    <t>MAX +</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>${description1}</t>
+  </si>
+  <si>
+    <t>${min1}</t>
+  </si>
+  <si>
+    <t>${measure1}</t>
+  </si>
+  <si>
+    <t>${notes1}</t>
+  </si>
+  <si>
+    <t>${description2}</t>
+  </si>
+  <si>
+    <t>${min2}</t>
+  </si>
+  <si>
+    <t>${measure2}</t>
+  </si>
+  <si>
+    <t>${description3}</t>
+  </si>
+  <si>
+    <t>${min3}</t>
+  </si>
+  <si>
+    <t>${measure3}</t>
+  </si>
+  <si>
+    <t>${description4}</t>
+  </si>
+  <si>
+    <t>${min4}</t>
+  </si>
+  <si>
+    <t>${measure4}</t>
+  </si>
+  <si>
+    <t>${description5}</t>
+  </si>
+  <si>
+    <t>${min5}</t>
+  </si>
+  <si>
+    <t>${measure5}</t>
+  </si>
+  <si>
+    <t>${description6}</t>
+  </si>
+  <si>
+    <t>${min6}</t>
+  </si>
+  <si>
+    <t>${measure6}</t>
+  </si>
+  <si>
+    <t>${description7}</t>
+  </si>
+  <si>
+    <t>${min7}</t>
+  </si>
+  <si>
+    <t>${measure7}</t>
+  </si>
+  <si>
+    <t>${description8}</t>
+  </si>
+  <si>
+    <t>${min8}</t>
+  </si>
+  <si>
+    <t>${measure8}</t>
+  </si>
+  <si>
+    <t>${description9}</t>
+  </si>
+  <si>
+    <t>${min9}</t>
+  </si>
+  <si>
+    <t>${measure9}</t>
+  </si>
+  <si>
+    <t>${description10}</t>
+  </si>
+  <si>
+    <t>${min10}</t>
+  </si>
+  <si>
+    <t>${measure10}</t>
+  </si>
+  <si>
+    <t>Visual Attributes</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ASDFASD</t>
+  </si>
+  <si>
+    <t>${notes2}</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
   <si>
     <t>Part Number:</t>
   </si>
   <si>
     <t>_______________________________________</t>
-  </si>
-  <si>
-    <t>REV 5-10-21</t>
-  </si>
-  <si>
-    <t>Part Revision:</t>
-  </si>
-  <si>
-    <t>Job #:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Approval: </t>
-  </si>
-  <si>
-    <t>Check Freq:</t>
-  </si>
-  <si>
-    <t>Measurable Attributes</t>
-  </si>
-  <si>
-    <t>Thousanths</t>
-  </si>
-  <si>
-    <t>Skid number &amp; time</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>MIN -</t>
-  </si>
-  <si>
-    <t>Measure=</t>
-  </si>
-  <si>
-    <t>MAX +</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>${measure1}</t>
-  </si>
-  <si>
-    <t>Visual Attributes</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>ASDFASD</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
   </si>
   <si>
     <t>Measure</t>
@@ -122,7 +230,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -131,6 +239,11 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -154,8 +267,17 @@
       <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +294,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDADADA"/>
         <bgColor rgb="FFDADADA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -277,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -285,29 +413,38 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -322,41 +459,59 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -610,6 +765,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
@@ -617,11 +775,11 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1"/>
@@ -631,14 +789,14 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -646,11 +804,11 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -661,11 +819,11 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -674,280 +832,335 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8">
-      <c r="E8" s="18"/>
-      <c r="L8" s="19"/>
+      <c r="E8" s="21"/>
+      <c r="L8" s="22"/>
     </row>
     <row r="9">
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="23">
-        <v>121.0</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="25"/>
+      <c r="A10" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="29"/>
     </row>
     <row r="12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="29"/>
     </row>
     <row r="13">
-      <c r="A13" s="5"/>
-      <c r="B13" s="23">
-        <v>123123.0</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="A13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="29"/>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="29"/>
     </row>
     <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="29"/>
     </row>
     <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="29"/>
     </row>
     <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="29"/>
     </row>
     <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="A18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="29"/>
     </row>
     <row r="19">
-      <c r="A19" s="5"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="29"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
+      <c r="A20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="17"/>
+      <c r="A21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
-      <c r="L22" s="19"/>
+      <c r="A22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="21"/>
+      <c r="L22" s="22"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="18"/>
-      <c r="L23" s="19"/>
+      <c r="A23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="21"/>
+      <c r="L23" s="22"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="18"/>
-      <c r="L24" s="19"/>
+      <c r="A24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="21"/>
+      <c r="L24" s="22"/>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="18"/>
-      <c r="L25" s="19"/>
+      <c r="A25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="21"/>
+      <c r="L25" s="22"/>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="18"/>
-      <c r="L26" s="19"/>
+      <c r="A26" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="21"/>
+      <c r="L26" s="22"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="18"/>
-      <c r="L27" s="19"/>
+      <c r="A27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="21"/>
+      <c r="L27" s="22"/>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="18"/>
-      <c r="L28" s="19"/>
+      <c r="A28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="21"/>
+      <c r="L28" s="22"/>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="18"/>
-      <c r="L29" s="19"/>
+      <c r="A29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="21"/>
+      <c r="L29" s="22"/>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="22"/>
+      <c r="A30" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1003,14 +1216,14 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
+      <c r="C1" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1032,14 +1245,14 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
+      <c r="D2" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="4"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1062,11 +1275,11 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1092,11 +1305,11 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1120,407 +1333,407 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
+      <c r="A6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>30</v>
+      <c r="A7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="28"/>
-      <c r="AA10" s="28"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="36"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="36"/>
     </row>
     <row r="11">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
-      <c r="X11" s="28"/>
-      <c r="Y11" s="28"/>
-      <c r="Z11" s="28"/>
-      <c r="AA11" s="28"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
     </row>
     <row r="12">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="28"/>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="28"/>
-      <c r="AA12" s="28"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="36"/>
     </row>
     <row r="13">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="Y14" s="28"/>
-      <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="36"/>
     </row>
     <row r="15">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="28"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="28"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="28"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="28"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="9"/>
+      <c r="A20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1607,7 +1820,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="31"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2152,17 +2365,17 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="C1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5"/>
+      <c r="I1" s="8"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2184,14 +2397,14 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2214,12 +2427,12 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2244,12 +2457,12 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2272,74 +2485,74 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
+      <c r="A6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>30</v>
+      <c r="A7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
optimizations and code refactoring
</commit_message>
<xml_diff>
--- a/public/excel/PreProduction/QC Documentation.xlsx
+++ b/public/excel/PreProduction/QC Documentation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>Par Name:</t>
   </si>
@@ -79,10 +79,10 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>${description1}</t>
-  </si>
-  <si>
-    <t>${min1}</t>
+    <t>${mes_attr_description1}</t>
+  </si>
+  <si>
+    <t>${mes_min1}</t>
   </si>
   <si>
     <t>${measure1}</t>
@@ -91,82 +91,82 @@
     <t>${notes1}</t>
   </si>
   <si>
-    <t>${description2}</t>
-  </si>
-  <si>
-    <t>${min2}</t>
+    <t>${mes_attr_description2}</t>
+  </si>
+  <si>
+    <t>${mes_min2}</t>
   </si>
   <si>
     <t>${measure2}</t>
   </si>
   <si>
-    <t>${description3}</t>
-  </si>
-  <si>
-    <t>${min3}</t>
+    <t>${mes_attr_description3}</t>
+  </si>
+  <si>
+    <t>${mes_min3}</t>
   </si>
   <si>
     <t>${measure3}</t>
   </si>
   <si>
-    <t>${description4}</t>
-  </si>
-  <si>
-    <t>${min4}</t>
+    <t>${mes_attr_description4}</t>
+  </si>
+  <si>
+    <t>${mes_min4}</t>
   </si>
   <si>
     <t>${measure4}</t>
   </si>
   <si>
-    <t>${description5}</t>
-  </si>
-  <si>
-    <t>${min5}</t>
+    <t>${mes_attr_description5}</t>
+  </si>
+  <si>
+    <t>${mes_min5}</t>
   </si>
   <si>
     <t>${measure5}</t>
   </si>
   <si>
-    <t>${description6}</t>
-  </si>
-  <si>
-    <t>${min6}</t>
+    <t>${mes_attr_description6}</t>
+  </si>
+  <si>
+    <t>${mes_min6}</t>
   </si>
   <si>
     <t>${measure6}</t>
   </si>
   <si>
-    <t>${description7}</t>
-  </si>
-  <si>
-    <t>${min7}</t>
+    <t>${mes_attr_description7}</t>
+  </si>
+  <si>
+    <t>${mes_min7}</t>
   </si>
   <si>
     <t>${measure7}</t>
   </si>
   <si>
-    <t>${description8}</t>
-  </si>
-  <si>
-    <t>${min8}</t>
+    <t>${mes_attr_description8}</t>
+  </si>
+  <si>
+    <t>${mes_min8}</t>
   </si>
   <si>
     <t>${measure8}</t>
   </si>
   <si>
-    <t>${description9}</t>
-  </si>
-  <si>
-    <t>${min9}</t>
+    <t>${mes_attr_description9}</t>
+  </si>
+  <si>
+    <t>${mes_min9}</t>
   </si>
   <si>
     <t>${measure9}</t>
   </si>
   <si>
-    <t>${description10}</t>
-  </si>
-  <si>
-    <t>${min10}</t>
+    <t>${mes_attr_description10}</t>
+  </si>
+  <si>
+    <t>${mes_min10}</t>
   </si>
   <si>
     <t>${measure10}</t>
@@ -175,46 +175,100 @@
     <t>Visual Attributes</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>ASDFASD</t>
+    <t>${vis_attr_description1}</t>
+  </si>
+  <si>
+    <t>${vis_min1}</t>
+  </si>
+  <si>
+    <t>${vis_mes1}</t>
   </si>
   <si>
     <t>${notes2}</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>j</t>
+    <t>${vis_attr_description2}</t>
+  </si>
+  <si>
+    <t>${vis_min2}</t>
+  </si>
+  <si>
+    <t>${vis_mes2}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description3}</t>
+  </si>
+  <si>
+    <t>${vis_min3}</t>
+  </si>
+  <si>
+    <t>${vis_mes3}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description4}</t>
+  </si>
+  <si>
+    <t>${vis_min4}</t>
+  </si>
+  <si>
+    <t>${vis_mes4}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description5}</t>
+  </si>
+  <si>
+    <t>${vis_min5}</t>
+  </si>
+  <si>
+    <t>${vis_mes5}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description6}</t>
+  </si>
+  <si>
+    <t>${vis_min6}</t>
+  </si>
+  <si>
+    <t>${vis_mes6}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description7}</t>
+  </si>
+  <si>
+    <t>${vis_min7}</t>
+  </si>
+  <si>
+    <t>${vis_mes7}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description8}</t>
+  </si>
+  <si>
+    <t>${vis_min8}</t>
+  </si>
+  <si>
+    <t>${vis_mes8}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description9}</t>
+  </si>
+  <si>
+    <t>${vis_min9}</t>
+  </si>
+  <si>
+    <t>${vis_mes9}</t>
+  </si>
+  <si>
+    <t>${vis_attr_description10}</t>
+  </si>
+  <si>
+    <t>${vis_min10}</t>
+  </si>
+  <si>
+    <t>${vis_mes10}</t>
   </si>
   <si>
     <t>Part Number:</t>
-  </si>
-  <si>
-    <t>_______________________________________</t>
   </si>
   <si>
     <t>Measure</t>
@@ -230,7 +284,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -239,11 +293,6 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -277,7 +326,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +349,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -415,16 +470,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -433,18 +485,18 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -459,60 +511,60 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,11 +827,11 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1"/>
@@ -789,14 +841,14 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -804,10 +856,10 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="1"/>
@@ -819,10 +871,10 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="1"/>
@@ -832,335 +884,373 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
     </row>
     <row r="8">
-      <c r="E8" s="21"/>
-      <c r="L8" s="22"/>
+      <c r="E8" s="20"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9">
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="28"/>
     </row>
     <row r="12">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="28"/>
     </row>
     <row r="16">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="20"/>
+        <v>54</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="21"/>
-      <c r="L22" s="22"/>
+      <c r="A22" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="20"/>
+      <c r="L22" s="21"/>
     </row>
     <row r="23">
-      <c r="A23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="21"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="20"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="21"/>
-      <c r="L24" s="22"/>
+      <c r="A24" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="20"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="21"/>
-      <c r="L25" s="22"/>
+      <c r="A25" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="20"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="21"/>
-      <c r="L26" s="22"/>
+      <c r="A26" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="20"/>
+      <c r="L26" s="21"/>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="21"/>
-      <c r="L27" s="22"/>
+      <c r="A27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="20"/>
+      <c r="L27" s="21"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="21"/>
-      <c r="L28" s="22"/>
+      <c r="A28" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="20"/>
+      <c r="L28" s="21"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="21"/>
-      <c r="L29" s="22"/>
+      <c r="A29" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="20"/>
+      <c r="L29" s="21"/>
     </row>
     <row r="30">
-      <c r="A30" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="25"/>
+      <c r="A30" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1209,6 +1299,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="22.29"/>
     <col customWidth="1" min="5" max="8" width="4.43"/>
     <col customWidth="1" min="9" max="27" width="4.0"/>
   </cols>
@@ -1216,14 +1307,17 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="5" t="s">
-        <v>63</v>
+      <c r="C1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="8"/>
+      <c r="J1" s="7"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1245,14 +1339,14 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>64</v>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1275,11 +1369,11 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1305,11 +1399,11 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1333,693 +1427,813 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B14" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="C14" s="37" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="36"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="36"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="36"/>
-      <c r="Z11" s="36"/>
-      <c r="AA11" s="36"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="36"/>
-      <c r="AA13" s="36"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="36"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="36"/>
+      <c r="A15" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="36"/>
+      <c r="A16" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
-      <c r="AA17" s="36"/>
+      <c r="A17" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="36"/>
+      <c r="A18" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="36"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
-      <c r="AA19" s="36"/>
+      <c r="A19" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="12"/>
+      <c r="A20" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
+      <c r="A21" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
+      <c r="A22" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
+      <c r="A23" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="1"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
+      <c r="A24" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
+      <c r="A25" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
+      <c r="A26" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
+      <c r="A27" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
+      <c r="A28" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
+      <c r="A29" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
+      <c r="A30" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
     </row>
     <row r="31">
       <c r="A31" s="1"/>
@@ -2365,17 +2579,16 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2397,14 +2610,13 @@
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="6"/>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2427,13 +2639,12 @@
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -2457,13 +2668,12 @@
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2485,74 +2695,76 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>66</v>
+      <c r="B7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -3760,13 +3972,17 @@
       <c r="Z52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:A9"/>
+  <mergeCells count="10">
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:Z9"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>